<commit_message>
Excel con los Modelos de contexto
</commit_message>
<xml_diff>
--- a/MuestreoDeDatosHojaDeVidaComputador.xlsx
+++ b/MuestreoDeDatosHojaDeVidaComputador.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Escritorio\Diseño Orientado a Objetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5537A753-877A-4F4B-835B-DD8330160207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5537A753-877A-4F4B-835B-DD8330160207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD51121B-62C6-486D-93D4-9CC6D0B12C6D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="18" xr2:uid="{B9480CE2-4DA4-4A08-8AF4-3893818E16B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="7" xr2:uid="{B9480CE2-4DA4-4A08-8AF4-3893818E16B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Institucion" sheetId="3" r:id="rId1"/>
@@ -615,9 +615,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -655,7 +655,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -761,7 +761,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -903,7 +903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1698,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5278083-1E8A-4703-8711-436F44BE2F0C}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +1871,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,15 +2330,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF4C3EB-6449-40CE-AF79-1EB9E570916B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>